<commit_message>
A file has been removed
</commit_message>
<xml_diff>
--- a/Pairwise (2).xlsx
+++ b/Pairwise (2).xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="516" yWindow="552" windowWidth="15996" windowHeight="6564"/>
   </bookViews>
   <sheets>
-    <sheet name="Pairwise" sheetId="1" r:id="rId4"/>
+    <sheet name="Pairwise" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="17">
   <si>
     <t>Вид животного</t>
   </si>
@@ -63,28 +62,23 @@
   </si>
   <si>
     <t>Кот</t>
+  </si>
+  <si>
+    <t>Собака</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -95,34 +89,40 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -412,28 +412,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -464,7 +461,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1">
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -481,7 +478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1">
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -498,7 +495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1">
+    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -515,7 +512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1">
+    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -532,7 +529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="2" customFormat="1">
+    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -549,7 +546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="2" customFormat="1">
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -566,7 +563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="2" customFormat="1">
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -583,12 +580,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="2" customFormat="1">
+    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -600,7 +597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="2" customFormat="1">
+    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -617,7 +614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="2" customFormat="1">
+    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -634,7 +631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="2" customFormat="1">
+    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -651,7 +648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="2" customFormat="1">
+    <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -668,7 +665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="2" customFormat="1">
+    <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -685,7 +682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="2" customFormat="1">
+    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -702,7 +699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="2" customFormat="1">
+    <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -719,7 +716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="2" customFormat="1">
+    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -736,7 +733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="2" customFormat="1">
+    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -753,7 +750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1">
+    <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -770,7 +767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="2" customFormat="1">
+    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -787,7 +784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="2" customFormat="1">
+    <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -804,7 +801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1">
+    <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -821,7 +818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="2" customFormat="1">
+    <row r="24" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -838,7 +835,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="2" customFormat="1">
+    <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -855,7 +852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="2" customFormat="1">
+    <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -872,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="2" customFormat="1">
+    <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -889,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="2" customFormat="1">
+    <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -906,7 +903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="2" customFormat="1">
+    <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -923,7 +920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="2" customFormat="1">
+    <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -940,7 +937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="2" customFormat="1">
+    <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -957,7 +954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="2" customFormat="1">
+    <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -975,17 +972,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>